<commit_message>
Update data for figure.
</commit_message>
<xml_diff>
--- a/examples/Memristor_Modeling/Generate_figure/P_variation.xlsx
+++ b/examples/Memristor_Modeling/Generate_figure/P_variation.xlsx
@@ -351,7 +351,7 @@
         <v>0.6706706285476685</v>
       </c>
       <c r="B1">
-        <v>2.022022008895874</v>
+        <v>0.9109108448028564</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -359,7 +359,7 @@
         <v>0.8208208084106445</v>
       </c>
       <c r="B2">
-        <v>1.981981873512268</v>
+        <v>0.8708708882331848</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -367,7 +367,7 @@
         <v>0.6506506204605103</v>
       </c>
       <c r="B3">
-        <v>2.052052021026611</v>
+        <v>0.9309308528900146</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -375,7 +375,7 @@
         <v>0.6406406164169312</v>
       </c>
       <c r="B4">
-        <v>2.06206202507019</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -383,7 +383,7 @@
         <v>0.7107107043266296</v>
       </c>
       <c r="B5">
-        <v>2.07207202911377</v>
+        <v>0.9109108448028564</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -391,7 +391,7 @@
         <v>0.6106106042861938</v>
       </c>
       <c r="B6">
-        <v>2.102102041244507</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -399,7 +399,7 @@
         <v>0.60060054063797</v>
       </c>
       <c r="B7">
-        <v>2.132132053375244</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -407,7 +407,7 @@
         <v>0.6306306123733521</v>
       </c>
       <c r="B8">
-        <v>2.132132053375244</v>
+        <v>0.9509509205818176</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -415,7 +415,7 @@
         <v>0.6106106042861938</v>
       </c>
       <c r="B9">
-        <v>2.122122049331665</v>
+        <v>0.9209208488464355</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -423,7 +423,7 @@
         <v>0.6406406164169312</v>
       </c>
       <c r="B10">
-        <v>2.112112045288086</v>
+        <v>0.9309308528900146</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -431,7 +431,7 @@
         <v>0.8108108043670654</v>
       </c>
       <c r="B11">
-        <v>2.152152061462402</v>
+        <v>0.9309308528900146</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -439,7 +439,7 @@
         <v>0.7407407164573669</v>
       </c>
       <c r="B12">
-        <v>2.132132053375244</v>
+        <v>0.9309308528900146</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -447,7 +447,7 @@
         <v>0.6406406164169312</v>
       </c>
       <c r="B13">
-        <v>2.162162065505981</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -455,7 +455,7 @@
         <v>0.6706706285476685</v>
       </c>
       <c r="B14">
-        <v>2.192192077636719</v>
+        <v>0.9609609246253967</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -463,7 +463,7 @@
         <v>0.7607607245445251</v>
       </c>
       <c r="B15">
-        <v>2.142142057418823</v>
+        <v>0.9309308528900146</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -471,7 +471,7 @@
         <v>0.750750720500946</v>
       </c>
       <c r="B16">
-        <v>2.202202081680298</v>
+        <v>0.9609609246253967</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -479,7 +479,7 @@
         <v>0.7107107043266296</v>
       </c>
       <c r="B17">
-        <v>2.212212085723877</v>
+        <v>0.9609609246253967</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -487,7 +487,7 @@
         <v>0.7007007002830505</v>
       </c>
       <c r="B18">
-        <v>2.18218207359314</v>
+        <v>0.9509509205818176</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -495,7 +495,7 @@
         <v>0.7007007002830505</v>
       </c>
       <c r="B19">
-        <v>2.18218207359314</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -503,7 +503,7 @@
         <v>0.6906906366348267</v>
       </c>
       <c r="B20">
-        <v>2.202202081680298</v>
+        <v>0.9309308528900146</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -511,7 +511,7 @@
         <v>0.7107107043266296</v>
       </c>
       <c r="B21">
-        <v>2.262262105941772</v>
+        <v>0.9809809327125549</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -519,7 +519,7 @@
         <v>0.6706706285476685</v>
       </c>
       <c r="B22">
-        <v>2.212212085723877</v>
+        <v>0.9209208488464355</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -527,7 +527,7 @@
         <v>0.6906906366348267</v>
       </c>
       <c r="B23">
-        <v>2.232232093811035</v>
+        <v>0.9509509205818176</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -535,7 +535,7 @@
         <v>0.7107107043266296</v>
       </c>
       <c r="B24">
-        <v>2.242242097854614</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -543,7 +543,7 @@
         <v>0.750750720500946</v>
       </c>
       <c r="B25">
-        <v>2.212212085723877</v>
+        <v>0.9309308528900146</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -551,7 +551,7 @@
         <v>0.7307307124137878</v>
       </c>
       <c r="B26">
-        <v>2.202202081680298</v>
+        <v>0.9009008407592773</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -559,7 +559,7 @@
         <v>0.7007007002830505</v>
       </c>
       <c r="B27">
-        <v>2.262262105941772</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -567,7 +567,7 @@
         <v>0.6706706285476685</v>
       </c>
       <c r="B28">
-        <v>2.252252101898193</v>
+        <v>0.9509509205818176</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -575,7 +575,7 @@
         <v>0.6906906366348267</v>
       </c>
       <c r="B29">
-        <v>2.232232093811035</v>
+        <v>0.9609609246253967</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -583,7 +583,7 @@
         <v>0.7107107043266296</v>
       </c>
       <c r="B30">
-        <v>2.232232093811035</v>
+        <v>0.9209208488464355</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -591,7 +591,7 @@
         <v>0.7407407164573669</v>
       </c>
       <c r="B31">
-        <v>2.222222089767456</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -599,7 +599,7 @@
         <v>0.750750720500946</v>
       </c>
       <c r="B32">
-        <v>2.222222089767456</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -607,7 +607,7 @@
         <v>0.750750720500946</v>
       </c>
       <c r="B33">
-        <v>2.222222089767456</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -615,7 +615,7 @@
         <v>0.7307307124137878</v>
       </c>
       <c r="B34">
-        <v>2.192192077636719</v>
+        <v>0.9209208488464355</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -623,7 +623,7 @@
         <v>0.750750720500946</v>
       </c>
       <c r="B35">
-        <v>2.202202081680298</v>
+        <v>0.9209208488464355</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -631,7 +631,7 @@
         <v>0.7307307124137878</v>
       </c>
       <c r="B36">
-        <v>2.202202081680298</v>
+        <v>0.9309308528900146</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -639,7 +639,7 @@
         <v>0.7407407164573669</v>
       </c>
       <c r="B37">
-        <v>2.222222089767456</v>
+        <v>0.9309308528900146</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -647,7 +647,7 @@
         <v>0.750750720500946</v>
       </c>
       <c r="B38">
-        <v>2.252252101898193</v>
+        <v>0.9309308528900146</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -655,7 +655,7 @@
         <v>0.7807807922363281</v>
       </c>
       <c r="B39">
-        <v>2.272272109985352</v>
+        <v>0.9509509205818176</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -663,7 +663,7 @@
         <v>0.7607607245445251</v>
       </c>
       <c r="B40">
-        <v>2.202202081680298</v>
+        <v>0.9209208488464355</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -671,7 +671,7 @@
         <v>0.7407407164573669</v>
       </c>
       <c r="B41">
-        <v>2.222222089767456</v>
+        <v>0.9309308528900146</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -679,7 +679,7 @@
         <v>0.770770788192749</v>
       </c>
       <c r="B42">
-        <v>2.212212085723877</v>
+        <v>0.9309308528900146</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -687,7 +687,7 @@
         <v>0.7207207083702087</v>
       </c>
       <c r="B43">
-        <v>2.222222089767456</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -695,7 +695,7 @@
         <v>0.7607607245445251</v>
       </c>
       <c r="B44">
-        <v>2.192192077636719</v>
+        <v>0.9309308528900146</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -703,7 +703,7 @@
         <v>0.8308308124542236</v>
       </c>
       <c r="B45">
-        <v>2.18218207359314</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -711,7 +711,7 @@
         <v>0.7307307124137878</v>
       </c>
       <c r="B46">
-        <v>2.192192077636719</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -719,7 +719,7 @@
         <v>0.7607607245445251</v>
       </c>
       <c r="B47">
-        <v>2.222222089767456</v>
+        <v>0.9609609246253967</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -727,7 +727,7 @@
         <v>0.7207207083702087</v>
       </c>
       <c r="B48">
-        <v>2.222222089767456</v>
+        <v>0.9709709286689758</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -735,7 +735,7 @@
         <v>0.7407407164573669</v>
       </c>
       <c r="B49">
-        <v>2.202202081680298</v>
+        <v>0.9509509205818176</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -743,7 +743,7 @@
         <v>0.7307307124137878</v>
       </c>
       <c r="B50">
-        <v>2.222222089767456</v>
+        <v>0.9509509205818176</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -751,7 +751,7 @@
         <v>0.7307307124137878</v>
       </c>
       <c r="B51">
-        <v>2.222222089767456</v>
+        <v>0.9609609246253967</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -759,7 +759,7 @@
         <v>0.7307307124137878</v>
       </c>
       <c r="B52">
-        <v>2.212212085723877</v>
+        <v>0.9509509205818176</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -767,7 +767,7 @@
         <v>0.7607607245445251</v>
       </c>
       <c r="B53">
-        <v>2.202202081680298</v>
+        <v>0.9409409165382385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>